<commit_message>
Ajout de module "resman"; documentation sur Generation et Analyse
</commit_message>
<xml_diff>
--- a/Result_analyse/Result.xlsx
+++ b/Result_analyse/Result.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zmdgd\source\repos\OpenMATB\Result_analyse\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38E2A2E4-F1C0-429E-BA41-3F902FA4D316}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BC2EF21-BBA8-4F02-86AA-E3ACFB37F518}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17040" yWindow="2955" windowWidth="21600" windowHeight="11385" xr2:uid="{41599D46-7C84-4631-BC73-87B7579C73F7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{41599D46-7C84-4631-BC73-87B7579C73F7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -84,8 +84,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="168" formatCode="0.000"/>
-    <numFmt numFmtId="169" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -141,13 +141,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -469,7 +469,7 @@
   <dimension ref="A1:O40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I37" sqref="A1:I37"/>
+      <selection activeCell="D4" sqref="D4:D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -661,6 +661,10 @@
       <c r="I6" s="2">
         <v>0.81005700000000003</v>
       </c>
+      <c r="O6">
+        <f>_xlfn.STDEV.P(F2:I37)</f>
+        <v>0.16718651608039148</v>
+      </c>
     </row>
     <row r="7" spans="1:15">
       <c r="B7">
@@ -1544,7 +1548,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E76025FD-153A-4A49-9536-223333469A1D}">
   <dimension ref="A1:K41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="K30" sqref="K30"/>
     </sheetView>
   </sheetViews>

</xml_diff>